<commit_message>
Final Code - Draft 2
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bujji/Documents/MS_SMU/Capstone/Capstone/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramya/Documents/GitHub/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B5AFCF-95FD-B04D-A6C7-9A3D71F98589}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="460" windowWidth="25660" windowHeight="14580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="42020" yWindow="4480" windowWidth="25660" windowHeight="14580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -22,12 +23,12 @@
     <sheet name="Question" sheetId="2" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">finalDataInputSheet!$A$3:$V$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">finalDataInputSheet!$A$1:$V$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">NewsApi!$A$1:$L$222</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="21" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -3648,9 +3649,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -3889,10 +3890,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3930,12 +3931,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43358.402759375" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="222">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43358.402759375" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="222" xr:uid="{00000000-000A-0000-FFFF-FFFF15000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H1048576" sheet="NewsApi"/>
   </cacheSource>
@@ -6237,7 +6241,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C23" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -6383,6 +6387,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -6650,7 +6657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -7005,11 +7012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8756,6 +8763,7 @@
       <c r="V41" s="30"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:V41" xr:uid="{0DE81900-AC6D-9F4B-83E8-444679808C78}"/>
   <sortState ref="A3:T39">
     <sortCondition descending="1" ref="B3:B39"/>
   </sortState>
@@ -8774,7 +8782,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -9318,57 +9326,57 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" tooltip="Democratic Party (United States)"/>
-    <hyperlink ref="B2" r:id="rId2" tooltip="Kamala Harris"/>
-    <hyperlink ref="A3" r:id="rId3" tooltip="Democratic Party (United States)"/>
-    <hyperlink ref="B3" r:id="rId4" tooltip="Loretta Sanchez"/>
-    <hyperlink ref="A4" r:id="rId5" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="B4" r:id="rId6" tooltip="George Sundheim"/>
-    <hyperlink ref="A5" r:id="rId7" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="B5" r:id="rId8" tooltip="Phil Wyman"/>
-    <hyperlink ref="A6" r:id="rId9" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="B6" r:id="rId10" tooltip="Tom Del Beccaro"/>
-    <hyperlink ref="A7" r:id="rId11" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="A8" r:id="rId12" tooltip="Democratic Party (United States)"/>
-    <hyperlink ref="A9" r:id="rId13" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="A10" r:id="rId14" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="A11" r:id="rId15" tooltip="Libertarian Party (United States)"/>
-    <hyperlink ref="A12" r:id="rId16" tooltip="Democratic Party (United States)"/>
-    <hyperlink ref="A13" r:id="rId17" tooltip="Green Party (United States)"/>
-    <hyperlink ref="A14" r:id="rId18" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="A15" r:id="rId19" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="B15" r:id="rId20" tooltip="Ron Unz"/>
-    <hyperlink ref="A16" r:id="rId21" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="A17" r:id="rId22" tooltip="No party preference"/>
-    <hyperlink ref="A18" r:id="rId23" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="A19" r:id="rId24" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="A20" r:id="rId25" tooltip="Democratic Party (United States)"/>
-    <hyperlink ref="A21" r:id="rId26" tooltip="Republican Party (United States)"/>
-    <hyperlink ref="A22" r:id="rId27" tooltip="Libertarian Party (United States)"/>
-    <hyperlink ref="B22" r:id="rId28" tooltip="Mark Matthew Herd"/>
-    <hyperlink ref="A23" r:id="rId29" tooltip="Peace and Freedom Party"/>
-    <hyperlink ref="A24" r:id="rId30" tooltip="No party preference"/>
-    <hyperlink ref="A25" r:id="rId31" tooltip="Democratic Party (United States)"/>
-    <hyperlink ref="A26" r:id="rId32" tooltip="Democratic Party (United States)"/>
-    <hyperlink ref="A27" r:id="rId33" tooltip="No party preference"/>
-    <hyperlink ref="A28" r:id="rId34" tooltip="No party preference"/>
-    <hyperlink ref="A29" r:id="rId35" tooltip="No party preference"/>
-    <hyperlink ref="A30" r:id="rId36" tooltip="No party preference"/>
-    <hyperlink ref="A31" r:id="rId37" tooltip="No party preference"/>
-    <hyperlink ref="A32" r:id="rId38" tooltip="No party preference"/>
-    <hyperlink ref="A33" r:id="rId39" tooltip="No party preference"/>
-    <hyperlink ref="A34" r:id="rId40" tooltip="No party preference"/>
-    <hyperlink ref="A35" r:id="rId41" tooltip="No party preference"/>
-    <hyperlink ref="A36" r:id="rId42" tooltip="Write-in candidate"/>
-    <hyperlink ref="A37" r:id="rId43" tooltip="Write-in candidate"/>
-    <hyperlink ref="A38" r:id="rId44" tooltip="Write-in candidate"/>
+    <hyperlink ref="A2" r:id="rId1" tooltip="Democratic Party (United States)" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" tooltip="Kamala Harris" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" tooltip="Democratic Party (United States)" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B3" r:id="rId4" tooltip="Loretta Sanchez" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="A4" r:id="rId5" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B4" r:id="rId6" tooltip="George Sundheim" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="A5" r:id="rId7" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B5" r:id="rId8" tooltip="Phil Wyman" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="A6" r:id="rId9" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B6" r:id="rId10" tooltip="Tom Del Beccaro" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="A7" r:id="rId11" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="A8" r:id="rId12" tooltip="Democratic Party (United States)" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="A9" r:id="rId13" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="A10" r:id="rId14" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="A11" r:id="rId15" tooltip="Libertarian Party (United States)" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="A12" r:id="rId16" tooltip="Democratic Party (United States)" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="A13" r:id="rId17" tooltip="Green Party (United States)" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="A14" r:id="rId18" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="A15" r:id="rId19" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="B15" r:id="rId20" tooltip="Ron Unz" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="A16" r:id="rId21" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="A17" r:id="rId22" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="A18" r:id="rId23" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="A19" r:id="rId24" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="A20" r:id="rId25" tooltip="Democratic Party (United States)" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="A21" r:id="rId26" tooltip="Republican Party (United States)" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="A22" r:id="rId27" tooltip="Libertarian Party (United States)" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="B22" r:id="rId28" tooltip="Mark Matthew Herd" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="A23" r:id="rId29" tooltip="Peace and Freedom Party" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="A24" r:id="rId30" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="A25" r:id="rId31" tooltip="Democratic Party (United States)" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="A26" r:id="rId32" tooltip="Democratic Party (United States)" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="A27" r:id="rId33" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="A28" r:id="rId34" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="A29" r:id="rId35" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="A30" r:id="rId36" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="A31" r:id="rId37" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="A32" r:id="rId38" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="A33" r:id="rId39" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="A34" r:id="rId40" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="A35" r:id="rId41" tooltip="No party preference" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="A36" r:id="rId42" tooltip="Write-in candidate" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="A37" r:id="rId43" tooltip="Write-in candidate" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="A38" r:id="rId44" tooltip="Write-in candidate" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9507,7 +9515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9560,7 +9568,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="384" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -9571,7 +9579,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -9582,7 +9590,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="384" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>98</v>
       </c>
@@ -9604,7 +9612,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -9626,7 +9634,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -9637,7 +9645,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="368" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="404" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -9659,7 +9667,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="336" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="372" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>103</v>
       </c>
@@ -9714,7 +9722,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>75</v>
       </c>
@@ -9736,7 +9744,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="336" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="372" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>115</v>
       </c>
@@ -9802,7 +9810,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>127</v>
       </c>
@@ -9813,7 +9821,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="368" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="404" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -9835,7 +9843,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="409" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>82</v>
       </c>
@@ -9885,7 +9893,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15778,7 +15786,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>13</v>
       </c>
@@ -16114,7 +16122,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>13</v>
       </c>
@@ -19146,13 +19154,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L222"/>
+  <autoFilter ref="A1:L222" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19508,7 +19516,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Code changes to Data Exploration
</commit_message>
<xml_diff>
--- a/DataSheet.xlsx
+++ b/DataSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramya/Documents/GitHub/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B5AFCF-95FD-B04D-A6C7-9A3D71F98589}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F3A06F-5444-224B-983F-FAADAB4415EE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42020" yWindow="4480" windowWidth="25660" windowHeight="14580" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="Question" sheetId="2" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">finalDataInputSheet!$A$1:$V$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">finalDataInputSheet!$A$3:$Y$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">NewsApi!$A$1:$L$222</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
@@ -7016,7 +7016,7 @@
   <dimension ref="A1:Y41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8763,7 +8763,7 @@
       <c r="V41" s="30"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V41" xr:uid="{0DE81900-AC6D-9F4B-83E8-444679808C78}"/>
+  <autoFilter ref="A3:Y41" xr:uid="{D15A8492-514D-E745-84C6-37D18E4C1175}"/>
   <sortState ref="A3:T39">
     <sortCondition descending="1" ref="B3:B39"/>
   </sortState>

</xml_diff>